<commit_message>
Suppression du jdv-localisation-anatomique-cisis (#79) a430e587395f144968b9eea886c79a2574c41837
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-fr-lm-quantite-exposition.xlsx
+++ b/main/ig/StructureDefinition-fr-lm-quantite-exposition.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-08T08:28:39+00:00</t>
+    <t>2025-12-10T16:53:25+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -319,7 +319,7 @@
     <t>Latéralité et topographie</t>
   </si>
   <si>
-    <t>jdv-localisation-anatomique-cisis (1.2.250.1.213.1.1.5.694)</t>
+    <t>SNOMED CT (2.16.840.1.113883.6.96)</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}

</xml_diff>